<commit_message>
Update clean macro-free Bound CRM Clean.xlsx template
</commit_message>
<xml_diff>
--- a/Bound CRM Clean.xlsx
+++ b/Bound CRM Clean.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidYong\Downloads\loyalty_card_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14EA6B04-452A-44C4-A668-3C290B45A9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F7FF7EC-1EAD-4200-91E8-1758B75DE2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{A688853C-F427-4FB2-906E-AD2E3F6823D5}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8FD4B3F8-8C4C-40F4-AF25-D9D5D98EF9E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,32 +42,26 @@
     <t>Unique ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Today's Order </t>
+    <t>Today's Order</t>
   </si>
   <si>
     <t>Total Orders</t>
   </si>
   <si>
-    <t>Tokens Earned</t>
-  </si>
-  <si>
-    <t>Tokens Redeemed</t>
+    <t>Token Earned</t>
+  </si>
+  <si>
+    <t>Token Redeemed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,24 +104,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{566A97FE-2C8E-4DD8-B67D-FBB9764C6992}" name="Table1" displayName="Table1" ref="A1:F304" totalsRowShown="0">
-  <autoFilter ref="A1:F304" xr:uid="{566A97FE-2C8E-4DD8-B67D-FBB9764C6992}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F304">
-    <sortCondition ref="D1:D304"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B0D74448-70AD-4BB0-8CF7-D4405E952F01}" name="Customer Name"/>
-    <tableColumn id="2" xr3:uid="{198FFD87-4411-4C0A-91EA-B3B7E933A679}" name="Unique ID"/>
-    <tableColumn id="3" xr3:uid="{7A45D1C9-E534-4684-8148-EEA77771F87C}" name="Today's Order "/>
-    <tableColumn id="4" xr3:uid="{4B86EE8A-C343-44DA-995E-5B877D502641}" name="Total Orders"/>
-    <tableColumn id="5" xr3:uid="{2A52720F-0373-431B-9AB3-20439AED0D59}" name="Tokens Earned"/>
-    <tableColumn id="6" xr3:uid="{3EE6EB16-15B8-4566-A7E2-8CB6B3AA6451}" name="Tokens Redeemed"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -426,25 +402,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38098108-F6FF-43BC-863D-757F940CC0C5}">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571A90F1-5590-4403-85D7-B5A78E9C4652}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.1328125" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.265625" customWidth="1"/>
-    <col min="6" max="6" width="18.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.59765625" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" customWidth="1"/>
-    <col min="9" max="10" width="15.53125" customWidth="1"/>
+    <col min="1" max="1" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -468,10 +440,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>